<commit_message>
v7.3: many updates according to changelog
</commit_message>
<xml_diff>
--- a/gearRatios.xlsx
+++ b/gearRatios.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacData/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F8EA92-36AF-EE47-947B-9BA41FCCE9DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDAB7E6-076F-D24C-A811-94B9E8118780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="5400" windowWidth="28240" windowHeight="17560" xr2:uid="{08C8DFDE-BC7B-7C49-809E-FAA34E1EF9B3}"/>
+    <workbookView xWindow="1220" yWindow="4060" windowWidth="28240" windowHeight="17560" xr2:uid="{08C8DFDE-BC7B-7C49-809E-FAA34E1EF9B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -378,7 +387,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,8 +408,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>B1*A$19</f>
-        <v>1.2</v>
+        <f t="shared" ref="B2:B16" si="0">B1*A$19</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -408,8 +417,8 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>B2*A$19</f>
-        <v>1.44</v>
+        <f t="shared" si="0"/>
+        <v>2.25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -417,8 +426,8 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>B3*A$19</f>
-        <v>1.728</v>
+        <f t="shared" si="0"/>
+        <v>3.375</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -426,8 +435,8 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>B4*A$19</f>
-        <v>2.0735999999999999</v>
+        <f t="shared" si="0"/>
+        <v>5.0625</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -435,8 +444,8 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <f>B5*A$19</f>
-        <v>2.4883199999999999</v>
+        <f t="shared" si="0"/>
+        <v>7.59375</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -444,8 +453,8 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <f>B6*A$19</f>
-        <v>2.9859839999999997</v>
+        <f t="shared" si="0"/>
+        <v>11.390625</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -453,8 +462,8 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <f>B7*A$19</f>
-        <v>3.5831807999999996</v>
+        <f t="shared" si="0"/>
+        <v>17.0859375</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -462,8 +471,8 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <f>B8*A$19</f>
-        <v>4.2998169599999994</v>
+        <f t="shared" si="0"/>
+        <v>25.62890625</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -471,8 +480,8 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <f>B9*A$19</f>
-        <v>5.1597803519999994</v>
+        <f t="shared" si="0"/>
+        <v>38.443359375</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -480,8 +489,8 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <f>B10*A$19</f>
-        <v>6.1917364223999991</v>
+        <f t="shared" si="0"/>
+        <v>57.6650390625</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -489,8 +498,8 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <f>B11*A$19</f>
-        <v>7.4300837068799988</v>
+        <f t="shared" si="0"/>
+        <v>86.49755859375</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -498,8 +507,8 @@
         <v>13</v>
       </c>
       <c r="B13" s="1">
-        <f>B12*A$19</f>
-        <v>8.9161004482559978</v>
+        <f t="shared" si="0"/>
+        <v>129.746337890625</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -507,8 +516,8 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <f>B13*A$19</f>
-        <v>10.699320537907196</v>
+        <f t="shared" si="0"/>
+        <v>194.6195068359375</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,8 +525,8 @@
         <v>15</v>
       </c>
       <c r="B15" s="1">
-        <f>B14*A$19</f>
-        <v>12.839184645488634</v>
+        <f t="shared" si="0"/>
+        <v>291.92926025390625</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -525,13 +534,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="1">
-        <f>B15*A$19</f>
-        <v>15.407021574586361</v>
+        <f t="shared" si="0"/>
+        <v>437.89389038085938</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>